<commit_message>
Monitoring variables validation done
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\OneDrive\Escritorio\trabajo\DSL\AdeptnessDSL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5362F548-D515-469B-B02A-2A850949899D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A8387C-DD9F-430E-9830-E176CE2F53DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B84BB494-B709-4470-B4D3-EE87A2BF8EE8}"/>
+    <workbookView xWindow="1692" yWindow="2832" windowWidth="17280" windowHeight="8964" xr2:uid="{B84BB494-B709-4470-B4D3-EE87A2BF8EE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,11 +128,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -290,15 +285,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -337,10 +332,6 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
@@ -354,19 +345,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,14 +431,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>182880</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1080" name="Check Box 56" hidden="1">
@@ -456,7 +452,7 @@
                   <a14:compatExt spid="_x0000_s1080"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB1B2362-ADEC-494D-B115-7129DD053993}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -496,20 +492,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>182880</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1081" name="Check Box 57" hidden="1">
@@ -518,7 +519,7 @@
                   <a14:compatExt spid="_x0000_s1081"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A91873CD-4685-4DA2-969B-A668A68D8074}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000039040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -558,20 +559,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>182880</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1082" name="Check Box 58" hidden="1">
@@ -580,7 +586,7 @@
                   <a14:compatExt spid="_x0000_s1082"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F04BEA0-D633-40D2-AC8E-EF7AD7F33468}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -620,20 +626,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>182880</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1083" name="Check Box 59" hidden="1">
@@ -642,7 +653,7 @@
                   <a14:compatExt spid="_x0000_s1083"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D196E76-865D-44AD-911B-98151CF6E449}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -682,20 +693,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>182880</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>198120</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1084" name="Check Box 60" hidden="1">
@@ -704,7 +720,7 @@
                   <a14:compatExt spid="_x0000_s1084"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2A9CC5D-5386-4880-A63C-B26DB629165B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -744,20 +760,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>182880</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1086" name="Check Box 62" hidden="1">
@@ -766,7 +787,7 @@
                   <a14:compatExt spid="_x0000_s1086"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F129C2A-965B-4271-993A-B761B11F7D6D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -806,7 +827,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -833,7 +854,7 @@
                   <a14:compatExt spid="_x0000_s1087"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54B7FD5C-E909-4ACF-90E1-BBC21F4B1BD9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -879,14 +900,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1088" name="Check Box 64" hidden="1">
@@ -895,7 +921,7 @@
                   <a14:compatExt spid="_x0000_s1088"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E587D936-74F8-49D3-BA8E-5A1B67CA8297}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000040040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -935,20 +961,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1089" name="Check Box 65" hidden="1">
@@ -957,7 +988,7 @@
                   <a14:compatExt spid="_x0000_s1089"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFFE7004-68B7-4CF5-8C0C-B87E47FD2D6C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000041040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -997,20 +1028,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1090" name="Check Box 66" hidden="1">
@@ -1019,7 +1055,7 @@
                   <a14:compatExt spid="_x0000_s1090"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A052FEF-83E4-4984-B67C-107245A8FDA2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1059,20 +1095,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1091" name="Check Box 67" hidden="1">
@@ -1081,7 +1122,7 @@
                   <a14:compatExt spid="_x0000_s1091"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33EBF22D-C8CB-49BD-B318-EB81D14BBADF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000043040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1121,20 +1162,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1094" name="Check Box 70" hidden="1">
@@ -1143,7 +1189,7 @@
                   <a14:compatExt spid="_x0000_s1094"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33B299EB-7083-40D5-A0DB-8531938C8BB4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000046040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1183,20 +1229,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1095" name="Check Box 71" hidden="1">
@@ -1205,7 +1256,7 @@
                   <a14:compatExt spid="_x0000_s1095"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0A8BF00-C032-4DE3-9CE0-CB25B70D2F2E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000047040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1245,29 +1296,34 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
-          <xdr:row>16</xdr:row>
+          <xdr:row>17</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1096" name="Check Box 72" hidden="1">
+            <xdr:cNvPr id="1097" name="Check Box 73" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1096"/>
+                  <a14:compatExt spid="_x0000_s1097"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E54E6FC2-F7B1-4248-A6B9-71AC525A5FE3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000049040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1307,29 +1363,34 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
-          <xdr:row>17</xdr:row>
+          <xdr:row>18</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1097" name="Check Box 73" hidden="1">
+            <xdr:cNvPr id="1098" name="Check Box 74" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1097"/>
+                  <a14:compatExt spid="_x0000_s1098"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72CA3A57-2B29-4D48-820F-10E73013B0D8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1369,29 +1430,34 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
-          <xdr:row>18</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1098" name="Check Box 74" hidden="1">
+            <xdr:cNvPr id="1100" name="Check Box 76" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1098"/>
+                  <a14:compatExt spid="_x0000_s1100"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB6BF0BE-B86F-4018-9A96-A189219491A9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1431,29 +1497,34 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1100" name="Check Box 76" hidden="1">
+            <xdr:cNvPr id="1101" name="Check Box 77" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1100"/>
+                  <a14:compatExt spid="_x0000_s1101"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04AD0CFC-B287-4E3B-9516-549D2959B6C2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1493,29 +1564,34 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
-          <xdr:row>21</xdr:row>
+          <xdr:row>23</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>25</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1101" name="Check Box 77" hidden="1">
+            <xdr:cNvPr id="1103" name="Check Box 79" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1101"/>
+                  <a14:compatExt spid="_x0000_s1103"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ECE37C4-7A6C-40F4-B491-A478D6314B37}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1555,29 +1631,34 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>251460</xdr:colOff>
-          <xdr:row>23</xdr:row>
+          <xdr:row>24</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>30480</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1103" name="Check Box 79" hidden="1">
+            <xdr:cNvPr id="1104" name="Check Box 80" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1103"/>
+                  <a14:compatExt spid="_x0000_s1104"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49AEA318-CFF6-47C9-A4AA-995517771E7E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000050040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1617,69 +1698,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>251460</xdr:colOff>
-          <xdr:row>24</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
-        </xdr:from>
-        <xdr:ext cx="571500" cy="213360"/>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1104" name="Check Box 80" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1104"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2902CD69-9722-40AD-A01A-022CCADCED16}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -1986,7 +2005,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2458,29 +2477,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1096" r:id="rId18" name="Check Box 72">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>251460</xdr:colOff>
-                    <xdr:row>16</xdr:row>
-                    <xdr:rowOff>190500</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>30480</xdr:colOff>
-                    <xdr:row>18</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1097" r:id="rId19" name="Check Box 73">
+            <control shapeId="1097" r:id="rId18" name="Check Box 73">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2502,7 +2499,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1098" r:id="rId20" name="Check Box 74">
+            <control shapeId="1098" r:id="rId19" name="Check Box 74">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2524,7 +2521,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1100" r:id="rId21" name="Check Box 76">
+            <control shapeId="1100" r:id="rId20" name="Check Box 76">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2546,7 +2543,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1101" r:id="rId22" name="Check Box 77">
+            <control shapeId="1101" r:id="rId21" name="Check Box 77">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2568,7 +2565,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1103" r:id="rId23" name="Check Box 79">
+            <control shapeId="1103" r:id="rId22" name="Check Box 79">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2590,7 +2587,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1104" r:id="rId24" name="Check Box 80">
+            <control shapeId="1104" r:id="rId23" name="Check Box 80">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>

</xml_diff>